<commit_message>
Tag 2 in Excel-Tabelle eingetragen
</commit_message>
<xml_diff>
--- a/Versuchsplan - Exp. 8 Drahtermüdung.xlsx
+++ b/Versuchsplan - Exp. 8 Drahtermüdung.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\baer-\Documents\GitHub\Ergebnisse-Zeitschaetzen\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{366921E3-94E3-4B59-BB00-B07B47813789}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4D8C25D-58EC-4B61-A400-C1962F9E02EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -109,7 +109,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -237,11 +237,48 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -281,6 +318,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -597,8 +642,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H49"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="91" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="G26" sqref="G26"/>
+    <sheetView tabSelected="1" topLeftCell="A24" zoomScale="91" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="G50" sqref="G50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.06640625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -904,28 +949,28 @@
       <c r="H12" s="1"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A13" s="5">
-        <v>12</v>
-      </c>
-      <c r="B13" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="C13" s="12">
+      <c r="A13" s="19">
+        <v>12</v>
+      </c>
+      <c r="B13" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="C13" s="21">
         <v>1</v>
       </c>
-      <c r="D13" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E13" s="2" t="s">
+      <c r="D13" s="22" t="s">
+        <v>7</v>
+      </c>
+      <c r="E13" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="F13" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G13" s="2">
-        <v>10</v>
-      </c>
-      <c r="H13" s="2"/>
+      <c r="F13" s="22" t="s">
+        <v>12</v>
+      </c>
+      <c r="G13" s="22">
+        <v>10</v>
+      </c>
+      <c r="H13" s="22"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A14" s="4">
@@ -1236,7 +1281,9 @@
       <c r="F26" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="G26" s="1"/>
+      <c r="G26" s="1">
+        <v>26</v>
+      </c>
       <c r="H26" s="1"/>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.45">
@@ -1258,7 +1305,9 @@
       <c r="F27" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="G27" s="2"/>
+      <c r="G27" s="2">
+        <v>9</v>
+      </c>
       <c r="H27" s="2"/>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.45">
@@ -1280,7 +1329,9 @@
       <c r="F28" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="G28" s="1"/>
+      <c r="G28" s="1">
+        <v>18</v>
+      </c>
       <c r="H28" s="1"/>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.45">
@@ -1302,7 +1353,9 @@
       <c r="F29" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="G29" s="2"/>
+      <c r="G29" s="2">
+        <v>9</v>
+      </c>
       <c r="H29" s="2"/>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.45">
@@ -1324,7 +1377,9 @@
       <c r="F30" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="G30" s="1"/>
+      <c r="G30" s="1">
+        <v>8</v>
+      </c>
       <c r="H30" s="1"/>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.45">
@@ -1346,7 +1401,9 @@
       <c r="F31" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="G31" s="2"/>
+      <c r="G31" s="2">
+        <v>42</v>
+      </c>
       <c r="H31" s="2"/>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.45">
@@ -1368,7 +1425,9 @@
       <c r="F32" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="G32" s="1"/>
+      <c r="G32" s="1">
+        <v>29</v>
+      </c>
       <c r="H32" s="1"/>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.45">
@@ -1390,7 +1449,9 @@
       <c r="F33" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="G33" s="2"/>
+      <c r="G33" s="2">
+        <v>31</v>
+      </c>
       <c r="H33" s="2"/>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.45">
@@ -1412,7 +1473,9 @@
       <c r="F34" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="G34" s="1"/>
+      <c r="G34" s="1">
+        <v>9</v>
+      </c>
       <c r="H34" s="1"/>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.45">
@@ -1434,7 +1497,9 @@
       <c r="F35" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="G35" s="2"/>
+      <c r="G35" s="2">
+        <v>13</v>
+      </c>
       <c r="H35" s="2"/>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.45">
@@ -1456,30 +1521,34 @@
       <c r="F36" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="G36" s="1"/>
+      <c r="G36" s="1">
+        <v>15</v>
+      </c>
       <c r="H36" s="1"/>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A37" s="5">
+      <c r="A37" s="19">
         <v>36</v>
       </c>
-      <c r="B37" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="C37" s="12">
+      <c r="B37" s="20" t="s">
+        <v>6</v>
+      </c>
+      <c r="C37" s="21">
         <v>3</v>
       </c>
-      <c r="D37" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E37" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F37" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G37" s="2"/>
-      <c r="H37" s="2"/>
+      <c r="D37" s="22" t="s">
+        <v>7</v>
+      </c>
+      <c r="E37" s="22" t="s">
+        <v>9</v>
+      </c>
+      <c r="F37" s="22" t="s">
+        <v>12</v>
+      </c>
+      <c r="G37" s="22">
+        <v>9</v>
+      </c>
+      <c r="H37" s="22"/>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A38" s="4">
@@ -1500,7 +1569,9 @@
       <c r="F38" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="G38" s="1"/>
+      <c r="G38" s="1">
+        <v>10</v>
+      </c>
       <c r="H38" s="1"/>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.45">
@@ -1522,7 +1593,9 @@
       <c r="F39" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="G39" s="2"/>
+      <c r="G39" s="2">
+        <v>9</v>
+      </c>
       <c r="H39" s="2"/>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.45">
@@ -1544,7 +1617,9 @@
       <c r="F40" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="G40" s="1"/>
+      <c r="G40" s="1">
+        <v>29</v>
+      </c>
       <c r="H40" s="1"/>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.45">
@@ -1566,7 +1641,9 @@
       <c r="F41" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="G41" s="2"/>
+      <c r="G41" s="2">
+        <v>9</v>
+      </c>
       <c r="H41" s="2"/>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.45">
@@ -1588,7 +1665,9 @@
       <c r="F42" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="G42" s="1"/>
+      <c r="G42" s="1">
+        <v>20</v>
+      </c>
       <c r="H42" s="1"/>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.45">
@@ -1610,7 +1689,9 @@
       <c r="F43" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="G43" s="2"/>
+      <c r="G43" s="2">
+        <v>16</v>
+      </c>
       <c r="H43" s="2"/>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.45">
@@ -1632,7 +1713,9 @@
       <c r="F44" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="G44" s="1"/>
+      <c r="G44" s="1">
+        <v>10</v>
+      </c>
       <c r="H44" s="1"/>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.45">
@@ -1654,7 +1737,9 @@
       <c r="F45" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="G45" s="2"/>
+      <c r="G45" s="2">
+        <v>8</v>
+      </c>
       <c r="H45" s="2"/>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.45">
@@ -1676,7 +1761,9 @@
       <c r="F46" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="G46" s="1"/>
+      <c r="G46" s="1">
+        <v>14</v>
+      </c>
       <c r="H46" s="1"/>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.45">
@@ -1698,7 +1785,9 @@
       <c r="F47" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="G47" s="2"/>
+      <c r="G47" s="2">
+        <v>18</v>
+      </c>
       <c r="H47" s="2"/>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.45">
@@ -1720,7 +1809,9 @@
       <c r="F48" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="G48" s="1"/>
+      <c r="G48" s="1">
+        <v>12</v>
+      </c>
       <c r="H48" s="1"/>
     </row>
     <row r="49" spans="1:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
@@ -1742,7 +1833,9 @@
       <c r="F49" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="G49" s="3"/>
+      <c r="G49" s="3">
+        <v>8</v>
+      </c>
       <c r="H49" s="3"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Drahtsorten in rot & silber im Versuchsprotokoll geändert
</commit_message>
<xml_diff>
--- a/Versuchsplan - Exp. 8 Drahtermüdung.xlsx
+++ b/Versuchsplan - Exp. 8 Drahtermüdung.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\baer-\Documents\GitHub\Ergebnisse-Zeitschaetzen\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4D8C25D-58EC-4B61-A400-C1962F9E02EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D962328-3B86-40C6-B65E-CDD52D7317D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -43,12 +43,6 @@
     <t>Tag 2</t>
   </si>
   <si>
-    <t>Eisen</t>
-  </si>
-  <si>
-    <t>Stahl</t>
-  </si>
-  <si>
     <t>ro-lu</t>
   </si>
   <si>
@@ -74,6 +68,12 @@
   </si>
   <si>
     <t>Wiederholungsmessung, Draht rausgerutscht</t>
+  </si>
+  <si>
+    <t>rot</t>
+  </si>
+  <si>
+    <t>silber</t>
   </si>
 </sst>
 </file>
@@ -109,7 +109,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="14">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -229,15 +229,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
       <left style="medium">
         <color indexed="64"/>
       </left>
@@ -278,7 +269,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -315,17 +306,14 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -642,8 +630,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" zoomScale="91" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="G50" sqref="G50"/>
+    <sheetView tabSelected="1" zoomScale="91" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.06640625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -658,7 +646,7 @@
   <sheetData>
     <row r="1" spans="1:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A1" s="14" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B1" s="15" t="s">
         <v>0</v>
@@ -676,10 +664,10 @@
         <v>4</v>
       </c>
       <c r="G1" s="16" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="H1" s="16" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.45">
@@ -693,13 +681,13 @@
         <v>1</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G2" s="1">
         <v>7</v>
@@ -717,13 +705,13 @@
         <v>1</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G3" s="2">
         <v>20</v>
@@ -741,13 +729,13 @@
         <v>1</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="G4" s="1">
         <v>22</v>
@@ -765,19 +753,19 @@
         <v>1</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="G5" s="2">
         <v>27</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.45">
@@ -791,13 +779,13 @@
         <v>1</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="G6" s="1">
         <v>8</v>
@@ -815,13 +803,13 @@
         <v>1</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="G7" s="2">
         <v>16</v>
@@ -832,20 +820,20 @@
       <c r="A8" s="4">
         <v>7</v>
       </c>
-      <c r="B8" s="18" t="s">
+      <c r="B8" s="8" t="s">
         <v>5</v>
       </c>
       <c r="C8" s="11">
         <v>1</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="G8" s="1">
         <v>7</v>
@@ -863,13 +851,13 @@
         <v>1</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G9" s="2">
         <v>10</v>
@@ -887,13 +875,13 @@
         <v>1</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G10" s="1">
         <v>34</v>
@@ -911,13 +899,13 @@
         <v>1</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="G11" s="2">
         <v>7</v>
@@ -935,13 +923,13 @@
         <v>1</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G12" s="1">
         <v>25</v>
@@ -949,28 +937,28 @@
       <c r="H12" s="1"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A13" s="19">
+      <c r="A13" s="18">
         <v>12</v>
       </c>
-      <c r="B13" s="20" t="s">
-        <v>5</v>
-      </c>
-      <c r="C13" s="21">
+      <c r="B13" s="19" t="s">
+        <v>5</v>
+      </c>
+      <c r="C13" s="20">
         <v>1</v>
       </c>
-      <c r="D13" s="22" t="s">
-        <v>7</v>
-      </c>
-      <c r="E13" s="22" t="s">
-        <v>11</v>
-      </c>
-      <c r="F13" s="22" t="s">
-        <v>12</v>
-      </c>
-      <c r="G13" s="22">
-        <v>10</v>
-      </c>
-      <c r="H13" s="22"/>
+      <c r="D13" s="21" t="s">
+        <v>16</v>
+      </c>
+      <c r="E13" s="21" t="s">
+        <v>9</v>
+      </c>
+      <c r="F13" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="G13" s="21">
+        <v>10</v>
+      </c>
+      <c r="H13" s="21"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A14" s="4">
@@ -983,13 +971,13 @@
         <v>2</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="G14" s="1">
         <v>13</v>
@@ -1007,13 +995,13 @@
         <v>2</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="G15" s="2">
         <v>8</v>
@@ -1031,13 +1019,13 @@
         <v>2</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G16" s="1">
         <v>10</v>
@@ -1055,13 +1043,13 @@
         <v>2</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G17" s="2">
         <v>9</v>
@@ -1079,13 +1067,13 @@
         <v>2</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="G18" s="1">
         <v>8</v>
@@ -1103,19 +1091,19 @@
         <v>2</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="G19" s="2">
         <v>15</v>
       </c>
       <c r="H19" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.45">
@@ -1129,13 +1117,13 @@
         <v>2</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G20" s="1">
         <v>24</v>
@@ -1153,13 +1141,13 @@
         <v>2</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G21" s="2">
         <v>17</v>
@@ -1177,13 +1165,13 @@
         <v>2</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="G22" s="1">
         <v>18</v>
@@ -1201,13 +1189,13 @@
         <v>2</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G23" s="2">
         <v>18</v>
@@ -1225,13 +1213,13 @@
         <v>2</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G24" s="1">
         <v>10</v>
@@ -1249,13 +1237,13 @@
         <v>2</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="F25" s="3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="G25" s="3">
         <v>9</v>
@@ -1273,13 +1261,13 @@
         <v>3</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G26" s="1">
         <v>26</v>
@@ -1297,13 +1285,13 @@
         <v>3</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="G27" s="2">
         <v>9</v>
@@ -1321,13 +1309,13 @@
         <v>3</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G28" s="1">
         <v>18</v>
@@ -1345,13 +1333,13 @@
         <v>3</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G29" s="2">
         <v>9</v>
@@ -1369,13 +1357,13 @@
         <v>3</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="G30" s="1">
         <v>8</v>
@@ -1393,13 +1381,13 @@
         <v>3</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="G31" s="2">
         <v>42</v>
@@ -1417,13 +1405,13 @@
         <v>3</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="G32" s="1">
         <v>29</v>
@@ -1441,13 +1429,13 @@
         <v>3</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="G33" s="2">
         <v>31</v>
@@ -1465,13 +1453,13 @@
         <v>3</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G34" s="1">
         <v>9</v>
@@ -1489,13 +1477,13 @@
         <v>3</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="G35" s="2">
         <v>13</v>
@@ -1513,13 +1501,13 @@
         <v>3</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G36" s="1">
         <v>15</v>
@@ -1527,28 +1515,28 @@
       <c r="H36" s="1"/>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A37" s="19">
+      <c r="A37" s="18">
         <v>36</v>
       </c>
-      <c r="B37" s="20" t="s">
-        <v>6</v>
-      </c>
-      <c r="C37" s="21">
+      <c r="B37" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="C37" s="20">
         <v>3</v>
       </c>
-      <c r="D37" s="22" t="s">
-        <v>7</v>
-      </c>
-      <c r="E37" s="22" t="s">
-        <v>9</v>
-      </c>
-      <c r="F37" s="22" t="s">
-        <v>12</v>
-      </c>
-      <c r="G37" s="22">
-        <v>9</v>
-      </c>
-      <c r="H37" s="22"/>
+      <c r="D37" s="21" t="s">
+        <v>16</v>
+      </c>
+      <c r="E37" s="21" t="s">
+        <v>7</v>
+      </c>
+      <c r="F37" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="G37" s="21">
+        <v>9</v>
+      </c>
+      <c r="H37" s="21"/>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A38" s="4">
@@ -1561,13 +1549,13 @@
         <v>4</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="G38" s="1">
         <v>10</v>
@@ -1585,13 +1573,13 @@
         <v>4</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="F39" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="G39" s="2">
         <v>9</v>
@@ -1609,13 +1597,13 @@
         <v>4</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="G40" s="1">
         <v>29</v>
@@ -1633,13 +1621,13 @@
         <v>4</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="E41" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F41" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G41" s="2">
         <v>9</v>
@@ -1657,13 +1645,13 @@
         <v>4</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="G42" s="1">
         <v>20</v>
@@ -1681,13 +1669,13 @@
         <v>4</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="E43" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F43" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G43" s="2">
         <v>16</v>
@@ -1705,13 +1693,13 @@
         <v>4</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="G44" s="1">
         <v>10</v>
@@ -1729,13 +1717,13 @@
         <v>4</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="E45" s="2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="F45" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G45" s="2">
         <v>8</v>
@@ -1753,13 +1741,13 @@
         <v>4</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G46" s="1">
         <v>14</v>
@@ -1777,13 +1765,13 @@
         <v>4</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="E47" s="2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="F47" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="G47" s="2">
         <v>18</v>
@@ -1801,13 +1789,13 @@
         <v>4</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="F48" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G48" s="1">
         <v>12</v>
@@ -1825,13 +1813,13 @@
         <v>4</v>
       </c>
       <c r="D49" s="3" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="E49" s="3" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="F49" s="3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G49" s="3">
         <v>8</v>

</xml_diff>